<commit_message>
5 year plan and Breakeven Analysis
</commit_message>
<xml_diff>
--- a/Paturo Docs/Paturo (BA and 5YP).xlsx
+++ b/Paturo Docs/Paturo (BA and 5YP).xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\TECHPRE-Project\Paturo Docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="6030"/>
   </bookViews>
   <sheets>
-    <sheet name="Breakeven Analysis" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="5 Year Plan" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
   <si>
     <t>Proforma Income Statement</t>
   </si>
@@ -85,28 +91,106 @@
     <t>Web Domain</t>
   </si>
   <si>
-    <t>Fixed Costs (per year)</t>
-  </si>
-  <si>
-    <t>Price (pesos)</t>
-  </si>
-  <si>
-    <t>Utilites (Internet Connection, Electricity, Water, etc)</t>
-  </si>
-  <si>
     <t>Advertising</t>
   </si>
   <si>
-    <t>ten employees</t>
-  </si>
-  <si>
-    <t>BREAKEVEN ANALYSIS</t>
-  </si>
-  <si>
-    <t>5 YEAR PLAN</t>
-  </si>
-  <si>
     <t>Revenue</t>
+  </si>
+  <si>
+    <t>Cost of Goods</t>
+  </si>
+  <si>
+    <t>Operating Expenses</t>
+  </si>
+  <si>
+    <t>Utilities</t>
+  </si>
+  <si>
+    <t>Subsciption</t>
+  </si>
+  <si>
+    <t>Servers</t>
+  </si>
+  <si>
+    <t>Total Revenue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Electricity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Internet</t>
+  </si>
+  <si>
+    <t>Total Operating Expenses</t>
+  </si>
+  <si>
+    <t>Total CoGS</t>
+  </si>
+  <si>
+    <t>Gross Profit</t>
+  </si>
+  <si>
+    <t>Gross Margin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          No. of tutoring sessions per user per month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Price per tutoring sessions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         Commision per month</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         Subsciption Fee per month</t>
+  </si>
+  <si>
+    <t>Net Income</t>
+  </si>
+  <si>
+    <t>SGA</t>
+  </si>
+  <si>
+    <t>5 Year Plan</t>
+  </si>
+  <si>
+    <t>5 year Growth Rate</t>
+  </si>
+  <si>
+    <t>Number of Users</t>
+  </si>
+  <si>
+    <t>Users Growth Rate</t>
+  </si>
+  <si>
+    <t>Credit Cart Processing Fee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Fixed Fee per Transaction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Transaction Percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Card Brand Transaction Percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Card Brand Fixed Fee</t>
+  </si>
+  <si>
+    <t>Comission</t>
+  </si>
+  <si>
+    <t>Advertisements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         Price per Click</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         Number of Clicks per month</t>
   </si>
 </sst>
 </file>
@@ -119,7 +203,7 @@
     <numFmt numFmtId="166" formatCode="[$$-409]#,##0.00"/>
     <numFmt numFmtId="167" formatCode="_([$PHP]\ * #,##0.00_);_([$PHP]\ * \(#,##0.00\);_([$PHP]\ * &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,6 +225,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="3">
@@ -181,11 +279,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -199,10 +298,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -472,7 +596,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -480,138 +604,645 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:Q55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="Q46" sqref="H46:Q53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="46.42578125" customWidth="1"/>
+    <col min="3" max="11" width="21.42578125" customWidth="1"/>
+    <col min="12" max="17" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="21"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="16"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="24">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="12">
+        <f>C5*C8*C9*C10*12</f>
+        <v>744000</v>
+      </c>
+      <c r="D7" s="12"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="12">
+        <v>500</v>
+      </c>
+      <c r="D9" s="12"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="C11" s="12">
+        <f>C5*C12*12</f>
+        <v>744000</v>
+      </c>
+      <c r="D11" s="12"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="12">
+        <v>100</v>
+      </c>
+      <c r="D12" s="12"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="12">
+        <f>C15*C14*12</f>
+        <v>223200</v>
+      </c>
+      <c r="D13" s="12"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="12">
+        <v>20</v>
+      </c>
+      <c r="D14" s="12"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="26">
+        <f>C5*1.5</f>
+        <v>930</v>
+      </c>
+      <c r="D15" s="12"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="16"/>
+      <c r="C16" s="17">
+        <f>C7+C11+C13</f>
+        <v>1711200</v>
+      </c>
+      <c r="D16" s="17"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="18"/>
+      <c r="C18" s="17">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="18"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="12">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="12">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="12">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="12">
+        <f>(C5*C8*C9*12*C25)+(C5*C8*C9*12*C27)+ (C5*C8*12*(C26+C28))</f>
+        <v>97464</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="25">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="25">
+        <v>1.1000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="16"/>
+      <c r="C29" s="17">
+        <f>C21+C22+C23</f>
+        <v>470000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="16"/>
+      <c r="C30" s="23">
+        <f>C29/C16</f>
+        <v>0.27466105656848994</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="16"/>
+      <c r="C31" s="17">
+        <f>C16-C29-C18</f>
+        <v>1191200</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="16"/>
+      <c r="C32" s="20">
+        <f>C31/C16</f>
+        <v>0.69611968209443664</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="18"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="12">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="12">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="C37" s="12">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" s="12">
+        <f>C39+C40+C41</f>
+        <v>147000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B39" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" s="15">
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B40" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40" s="15">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B41" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C41" s="15">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A42" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B42" s="18"/>
+      <c r="C42" s="17">
+        <f>C35+C36+C37+C38</f>
+        <v>897000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A44" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" s="17">
+        <f>C31 - C42</f>
+        <v>294200</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
+      <c r="F46">
+        <v>4</v>
+      </c>
+      <c r="G46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="12">
-        <f>SUM(B5,B6,B7,B8,B9,B10,B11)</f>
-        <v>2346000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="12">
-        <v>350000</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="12">
-        <v>400000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="12">
-        <v>240000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="12">
-        <v>250000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="C47" s="12">
+        <f>($C$5*($C$6+1)^(C46-1)*$C$8*$C$9*$C$10*12) + ($C$5*($C$6+1)^(C46-1)*$C$12*12)+ ($C$5*($C$6+1)^(C46-1)*1.5*C14*12)</f>
+        <v>1711200</v>
+      </c>
+      <c r="D47" s="12">
+        <f>($C$5*($C$6+1)^(D46-1)*$C$8*$C$9*$C$10*12) + ($C$5*($C$6+1)^(D46-1)*$C$12*12)+ ($C$5*($C$6+1)^(D46-1)*1.5*$C$14*12)</f>
+        <v>1882320</v>
+      </c>
+      <c r="E47" s="12">
+        <f t="shared" ref="E47:G47" si="0">($C$5*($C$6+1)^(E46-1)*$C$8*$C$9*$C$10*12) + ($C$5*($C$6+1)^(E46-1)*$C$12*12)+ ($C$5*($C$6+1)^(E46-1)*1.5*$C$14*12)</f>
+        <v>2070552.0000000005</v>
+      </c>
+      <c r="F47" s="12">
+        <f t="shared" si="0"/>
+        <v>2277607.2000000007</v>
+      </c>
+      <c r="G47" s="12">
+        <f t="shared" si="0"/>
+        <v>2505367.9200000009</v>
+      </c>
+      <c r="H47" s="12"/>
+      <c r="I47" s="12"/>
+      <c r="J47" s="12"/>
+      <c r="K47" s="12"/>
+      <c r="L47" s="12"/>
+      <c r="M47" s="12"/>
+      <c r="N47" s="12"/>
+      <c r="O47" s="12"/>
+      <c r="P47" s="12"/>
+      <c r="Q47" s="12"/>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" s="12">
+        <f>C47*$C$30</f>
+        <v>470000</v>
+      </c>
+      <c r="D48" s="12">
+        <f>D47*$C$30</f>
+        <v>517000</v>
+      </c>
+      <c r="E48" s="12">
+        <f t="shared" ref="E48:G48" si="1">E47*$C$30</f>
+        <v>568700.00000000012</v>
+      </c>
+      <c r="F48" s="12">
+        <f t="shared" si="1"/>
+        <v>625570.00000000012</v>
+      </c>
+      <c r="G48" s="12">
+        <f t="shared" si="1"/>
+        <v>688127.00000000023</v>
+      </c>
+      <c r="H48" s="12"/>
+      <c r="I48" s="12"/>
+      <c r="J48" s="12"/>
+      <c r="K48" s="12"/>
+      <c r="L48" s="12"/>
+      <c r="M48" s="12"/>
+      <c r="N48" s="12"/>
+      <c r="O48" s="12"/>
+      <c r="P48" s="12"/>
+      <c r="Q48" s="12"/>
+    </row>
+    <row r="49" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>41</v>
+      </c>
+      <c r="C49" s="12">
+        <v>0</v>
+      </c>
+      <c r="D49" s="12">
+        <v>0</v>
+      </c>
+      <c r="E49" s="12">
+        <v>0</v>
+      </c>
+      <c r="F49" s="12">
+        <v>0</v>
+      </c>
+      <c r="G49" s="12">
+        <v>0</v>
+      </c>
+      <c r="H49" s="12"/>
+      <c r="I49" s="12"/>
+      <c r="J49" s="12"/>
+      <c r="K49" s="12"/>
+      <c r="L49" s="12"/>
+      <c r="M49" s="12"/>
+      <c r="N49" s="12"/>
+      <c r="O49" s="12"/>
+      <c r="P49" s="12"/>
+      <c r="Q49" s="12"/>
+    </row>
+    <row r="50" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50" s="12">
+        <f>$C$18</f>
+        <v>50000</v>
+      </c>
+      <c r="D50" s="12">
+        <f>$C$18</f>
+        <v>50000</v>
+      </c>
+      <c r="E50" s="12">
+        <f t="shared" ref="E50:Q50" si="2">$C$18</f>
+        <v>50000</v>
+      </c>
+      <c r="F50" s="12">
+        <f t="shared" si="2"/>
+        <v>50000</v>
+      </c>
+      <c r="G50" s="12">
+        <f t="shared" si="2"/>
+        <v>50000</v>
+      </c>
+      <c r="H50" s="12"/>
+      <c r="I50" s="12"/>
+      <c r="J50" s="12"/>
+      <c r="K50" s="12"/>
+      <c r="L50" s="12"/>
+      <c r="M50" s="12"/>
+      <c r="N50" s="12"/>
+      <c r="O50" s="12"/>
+      <c r="P50" s="12"/>
+      <c r="Q50" s="12"/>
+    </row>
+    <row r="51" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>34</v>
+      </c>
+      <c r="C51" s="12">
+        <f>$C$47-$C$48-$C$49-$C$50</f>
+        <v>1191200</v>
+      </c>
+      <c r="D51" s="12">
+        <f>D47-D48-D49-D50</f>
+        <v>1315320</v>
+      </c>
+      <c r="E51" s="12">
+        <f t="shared" ref="E51:G51" si="3">E47-E48-E49-E50</f>
+        <v>1451852.0000000005</v>
+      </c>
+      <c r="F51" s="12">
+        <f t="shared" si="3"/>
+        <v>1602037.2000000007</v>
+      </c>
+      <c r="G51" s="12">
+        <f t="shared" si="3"/>
+        <v>1767240.9200000006</v>
+      </c>
+      <c r="H51" s="12"/>
+      <c r="I51" s="12"/>
+      <c r="J51" s="12"/>
+      <c r="K51" s="12"/>
+      <c r="L51" s="12"/>
+      <c r="M51" s="12"/>
+      <c r="N51" s="12"/>
+      <c r="O51" s="12"/>
+      <c r="P51" s="12"/>
+      <c r="Q51" s="12"/>
+    </row>
+    <row r="52" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="12">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="12">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="12">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>2</v>
-      </c>
-      <c r="E15">
-        <v>3</v>
-      </c>
-      <c r="F15">
-        <v>4</v>
-      </c>
-      <c r="G15">
-        <v>5</v>
+      <c r="C52" s="12">
+        <f>$C$42</f>
+        <v>897000</v>
+      </c>
+      <c r="D52" s="12">
+        <f>$C$42</f>
+        <v>897000</v>
+      </c>
+      <c r="E52" s="12">
+        <f t="shared" ref="E52:Q52" si="4">$C$42</f>
+        <v>897000</v>
+      </c>
+      <c r="F52" s="12">
+        <f t="shared" si="4"/>
+        <v>897000</v>
+      </c>
+      <c r="G52" s="12">
+        <f t="shared" si="4"/>
+        <v>897000</v>
+      </c>
+      <c r="H52" s="12"/>
+      <c r="I52" s="12"/>
+      <c r="J52" s="12"/>
+      <c r="K52" s="12"/>
+      <c r="L52" s="12"/>
+      <c r="M52" s="12"/>
+      <c r="N52" s="12"/>
+      <c r="O52" s="12"/>
+      <c r="P52" s="12"/>
+      <c r="Q52" s="12"/>
+    </row>
+    <row r="53" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C53" s="17">
+        <f>C51-C52</f>
+        <v>294200</v>
+      </c>
+      <c r="D53" s="17">
+        <f>D51-D52</f>
+        <v>418320</v>
+      </c>
+      <c r="E53" s="17">
+        <f t="shared" ref="E53:G53" si="5">E51-E52</f>
+        <v>554852.00000000047</v>
+      </c>
+      <c r="F53" s="17">
+        <f t="shared" si="5"/>
+        <v>705037.20000000065</v>
+      </c>
+      <c r="G53" s="17">
+        <f t="shared" si="5"/>
+        <v>870240.92000000062</v>
+      </c>
+      <c r="H53" s="17"/>
+      <c r="I53" s="17"/>
+      <c r="J53" s="17"/>
+      <c r="K53" s="17"/>
+      <c r="L53" s="17"/>
+      <c r="M53" s="17"/>
+      <c r="N53" s="17"/>
+      <c r="O53" s="17"/>
+      <c r="P53" s="17"/>
+      <c r="Q53" s="17"/>
+    </row>
+    <row r="55" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B55" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C55" s="20">
+        <f>$G$47/$C$47</f>
+        <v>1.4641000000000004</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A16:B16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>

</xml_diff>